<commit_message>
fix female life table age 100
</commit_message>
<xml_diff>
--- a/data/life_tables/ssa_ac_mort.xlsx
+++ b/data/life_tables/ssa_ac_mort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescalim/Documents/Documents - Francesca’s MacBook Pro/hire/multicancer_model/repo/HIRE-Multi-Cancer/data/life_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E004F94-C88D-ED42-B154-682B619B87FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA27D3-CBFF-E149-90E4-761420E3C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="1320" windowWidth="19360" windowHeight="17440" activeTab="1" xr2:uid="{3EC56884-69FF-7542-B150-5688BC92A570}"/>
+    <workbookView xWindow="19040" yWindow="500" windowWidth="19360" windowHeight="16240" activeTab="1" xr2:uid="{3EC56884-69FF-7542-B150-5688BC92A570}"/>
   </bookViews>
   <sheets>
     <sheet name="am" sheetId="1" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450C8A79-278A-E342-8826-692BF795288B}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3531,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E112591-F28E-9848-AB47-D485089FD743}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5462,10 +5462,10 @@
         <v>1</v>
       </c>
       <c r="C102" s="2">
-        <v>3410</v>
+        <v>0</v>
       </c>
       <c r="D102" s="2">
-        <v>3410</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2">
         <v>0</v>
@@ -5653,9 +5653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED03F1F2-757D-2E41-B40F-EA69F66C920E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
starter calibration code + cancer incidence
</commit_message>
<xml_diff>
--- a/data/life_tables/ssa_ac_mort.xlsx
+++ b/data/life_tables/ssa_ac_mort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescalim/Documents/Documents - Francesca’s MacBook Pro/hire/multicancer_model/repo/HIRE-Multi-Cancer/data/life_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E004F94-C88D-ED42-B154-682B619B87FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA27D3-CBFF-E149-90E4-761420E3C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="1320" windowWidth="19360" windowHeight="17440" activeTab="1" xr2:uid="{3EC56884-69FF-7542-B150-5688BC92A570}"/>
+    <workbookView xWindow="19040" yWindow="500" windowWidth="19360" windowHeight="16240" activeTab="1" xr2:uid="{3EC56884-69FF-7542-B150-5688BC92A570}"/>
   </bookViews>
   <sheets>
     <sheet name="am" sheetId="1" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450C8A79-278A-E342-8826-692BF795288B}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3531,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E112591-F28E-9848-AB47-D485089FD743}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5462,10 +5462,10 @@
         <v>1</v>
       </c>
       <c r="C102" s="2">
-        <v>3410</v>
+        <v>0</v>
       </c>
       <c r="D102" s="2">
-        <v>3410</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2">
         <v>0</v>
@@ -5653,9 +5653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED03F1F2-757D-2E41-B40F-EA69F66C920E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>